<commit_message>
tests: refactor test_query_error, process_test_config
</commit_message>
<xml_diff>
--- a/src/yarm/tests_data/test_queries_options/output/test.xlsx
+++ b/src/yarm/tests_data/test_queries_options/output/test.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Order Information" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Query A" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,108 +434,19 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>order_id</t>
+          <t>discount</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>product_id</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
           <t>name</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>discount</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="C2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Retro Time Machine</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="n">
-        <v>1000</v>
-      </c>
-      <c r="C3" t="n">
-        <v>2</v>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Replacement Crystals</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="n">
-        <v>1001</v>
-      </c>
-      <c r="C4" t="n">
-        <v>2</v>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Replacement Crystals</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="n">
-        <v>1001</v>
-      </c>
-      <c r="C5" t="n">
-        <v>3</v>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>D-QWON'S DANCE GROOVES (VHS)</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>0.75</t>
         </is>
       </c>
     </row>

</xml_diff>